<commit_message>
Modif demandée par Sébastien pour métriques discriminantes
</commit_message>
<xml_diff>
--- a/Métriques discriminantes/Tableau métriques/moyenne/2021_2022/Skill Corner/metrique_physical.xlsx
+++ b/Métriques discriminantes/Tableau métriques/moyenne/2021_2022/Skill Corner/metrique_physical.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA21"/>
+  <dimension ref="A1:AO21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,130 +441,200 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>total_distance_full_all</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>total_metersperminute_full_all</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>running_distance_full_all</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>hsr_distance_full_all</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>hsr_count_full_all</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>sprint_distance_full_all</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>sprint_count_full_all</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>hi_distance_full_all</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>hi_count_full_all</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>medaccel_count_full_all</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>highaccel_count_full_all</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>meddecel_count_full_all</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>highdecel_count_full_all</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>psv99</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
           <t>total_distance_full_tip</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>total_metersperminute_full_tip</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>running_distance_full_tip</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>hsr_distance_full_tip</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>hsr_count_full_tip</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>sprint_distance_full_tip</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>sprint_count_full_tip</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>hi_distance_full_tip</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>hi_count_full_tip</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>medaccel_count_full_tip</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>highaccel_count_full_tip</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>meddecel_count_full_tip</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>highdecel_count_full_tip</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>total_distance_full_otip</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>total_metersperminute_full_otip</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>running_distance_full_otip</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>hsr_distance_full_otip</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>hsr_count_full_otip</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>sprint_distance_full_otip</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>sprint_count_full_otip</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>hi_distance_full_otip</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>hi_count_full_otip</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>medaccel_count_full_otip</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>highaccel_count_full_otip</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>meddecel_count_full_otip</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>highdecel_count_full_otip</t>
         </is>
@@ -577,81 +647,123 @@
         </is>
       </c>
       <c r="B2" t="n">
+        <v>101246.1329588163</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1453.455315843169</v>
+      </c>
+      <c r="D2" t="n">
+        <v>14064.2079153171</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5375.009235331764</v>
+      </c>
+      <c r="F2" t="n">
+        <v>503.903269369846</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1612.107887889966</v>
+      </c>
+      <c r="H2" t="n">
+        <v>90.08759838775489</v>
+      </c>
+      <c r="I2" t="n">
+        <v>6987.11712322173</v>
+      </c>
+      <c r="J2" t="n">
+        <v>593.990867757601</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1026.938123561755</v>
+      </c>
+      <c r="L2" t="n">
+        <v>68.60283618067439</v>
+      </c>
+      <c r="M2" t="n">
+        <v>843.3616988811526</v>
+      </c>
+      <c r="N2" t="n">
+        <v>145.9082808155563</v>
+      </c>
+      <c r="O2" t="n">
+        <v>355.5818890191837</v>
+      </c>
+      <c r="P2" t="n">
         <v>38245.03311329238</v>
       </c>
-      <c r="C2" t="n">
+      <c r="Q2" t="n">
         <v>1757.557135943058</v>
       </c>
-      <c r="D2" t="n">
+      <c r="R2" t="n">
         <v>6200.304207411717</v>
       </c>
-      <c r="E2" t="n">
+      <c r="S2" t="n">
         <v>2381.49433727492</v>
       </c>
-      <c r="F2" t="n">
+      <c r="T2" t="n">
         <v>221.5532468662895</v>
       </c>
-      <c r="G2" t="n">
+      <c r="U2" t="n">
         <v>847.4837575814532</v>
       </c>
-      <c r="H2" t="n">
+      <c r="V2" t="n">
         <v>40.89049071784314</v>
       </c>
-      <c r="I2" t="n">
+      <c r="W2" t="n">
         <v>3228.978094856374</v>
       </c>
-      <c r="J2" t="n">
+      <c r="X2" t="n">
         <v>262.4437375841327</v>
       </c>
-      <c r="K2" t="n">
+      <c r="Y2" t="n">
         <v>384.5313542794729</v>
       </c>
-      <c r="L2" t="n">
+      <c r="Z2" t="n">
         <v>25.17144328777763</v>
       </c>
-      <c r="M2" t="n">
+      <c r="AA2" t="n">
         <v>276.9310007360748</v>
       </c>
-      <c r="N2" t="n">
+      <c r="AB2" t="n">
         <v>39.70680705549299</v>
       </c>
-      <c r="O2" t="n">
+      <c r="AC2" t="n">
         <v>31440.17263207441</v>
       </c>
-      <c r="P2" t="n">
+      <c r="AD2" t="n">
         <v>1891.126053113459</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="AE2" t="n">
         <v>6189.874009047865</v>
       </c>
-      <c r="R2" t="n">
+      <c r="AF2" t="n">
         <v>2532.094338317329</v>
       </c>
-      <c r="S2" t="n">
+      <c r="AG2" t="n">
         <v>222.136886035803</v>
       </c>
-      <c r="T2" t="n">
+      <c r="AH2" t="n">
         <v>621.4769208533244</v>
       </c>
-      <c r="U2" t="n">
+      <c r="AI2" t="n">
         <v>31.67411357577021</v>
       </c>
-      <c r="V2" t="n">
+      <c r="AJ2" t="n">
         <v>3153.571259170653</v>
       </c>
-      <c r="W2" t="n">
+      <c r="AK2" t="n">
         <v>253.8109996115732</v>
       </c>
-      <c r="X2" t="n">
+      <c r="AL2" t="n">
         <v>343.6188554092861</v>
       </c>
-      <c r="Y2" t="n">
+      <c r="AM2" t="n">
         <v>19.35495179734423</v>
       </c>
-      <c r="Z2" t="n">
+      <c r="AN2" t="n">
         <v>246.6065971555531</v>
       </c>
-      <c r="AA2" t="n">
+      <c r="AO2" t="n">
         <v>43.64389993789622</v>
       </c>
     </row>
@@ -662,81 +774,123 @@
         </is>
       </c>
       <c r="B3" t="n">
+        <v>102631.618022524</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1466.309969975657</v>
+      </c>
+      <c r="D3" t="n">
+        <v>14366.55457156884</v>
+      </c>
+      <c r="E3" t="n">
+        <v>5020.010256551216</v>
+      </c>
+      <c r="F3" t="n">
+        <v>488.9290768311829</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1311.192578310617</v>
+      </c>
+      <c r="H3" t="n">
+        <v>81.61987165380916</v>
+      </c>
+      <c r="I3" t="n">
+        <v>6331.202834861832</v>
+      </c>
+      <c r="J3" t="n">
+        <v>570.5489484849921</v>
+      </c>
+      <c r="K3" t="n">
+        <v>1027.048728612463</v>
+      </c>
+      <c r="L3" t="n">
+        <v>63.87237112033118</v>
+      </c>
+      <c r="M3" t="n">
+        <v>839.751211908086</v>
+      </c>
+      <c r="N3" t="n">
+        <v>147.6724120858165</v>
+      </c>
+      <c r="O3" t="n">
+        <v>349.7260742017392</v>
+      </c>
+      <c r="P3" t="n">
         <v>32499.04413726227</v>
       </c>
-      <c r="C3" t="n">
+      <c r="Q3" t="n">
         <v>1786.609670827545</v>
       </c>
-      <c r="D3" t="n">
+      <c r="R3" t="n">
         <v>5378.734706132076</v>
       </c>
-      <c r="E3" t="n">
+      <c r="S3" t="n">
         <v>2007.90645452699</v>
       </c>
-      <c r="F3" t="n">
+      <c r="T3" t="n">
         <v>195.3979334832982</v>
       </c>
-      <c r="G3" t="n">
+      <c r="U3" t="n">
         <v>617.2524073440741</v>
       </c>
-      <c r="H3" t="n">
+      <c r="V3" t="n">
         <v>33.34520400626526</v>
       </c>
-      <c r="I3" t="n">
+      <c r="W3" t="n">
         <v>2625.158861871064</v>
       </c>
-      <c r="J3" t="n">
+      <c r="X3" t="n">
         <v>228.7431374895635</v>
       </c>
-      <c r="K3" t="n">
+      <c r="Y3" t="n">
         <v>336.8281547835174</v>
       </c>
-      <c r="L3" t="n">
+      <c r="Z3" t="n">
         <v>21.20098980071841</v>
       </c>
-      <c r="M3" t="n">
+      <c r="AA3" t="n">
         <v>234.4034127069872</v>
       </c>
-      <c r="N3" t="n">
+      <c r="AB3" t="n">
         <v>37.37377923268704</v>
       </c>
-      <c r="O3" t="n">
+      <c r="AC3" t="n">
         <v>36289.31985932789</v>
       </c>
-      <c r="P3" t="n">
+      <c r="AD3" t="n">
         <v>1900.827443428021</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="AE3" t="n">
         <v>7294.948835296573</v>
       </c>
-      <c r="R3" t="n">
+      <c r="AF3" t="n">
         <v>2551.357721439193</v>
       </c>
-      <c r="S3" t="n">
+      <c r="AG3" t="n">
         <v>234.3660304445436</v>
       </c>
-      <c r="T3" t="n">
+      <c r="AH3" t="n">
         <v>566.7822713398243</v>
       </c>
-      <c r="U3" t="n">
+      <c r="AI3" t="n">
         <v>31.4896106465157</v>
       </c>
-      <c r="V3" t="n">
+      <c r="AJ3" t="n">
         <v>3118.139992779018</v>
       </c>
-      <c r="W3" t="n">
+      <c r="AK3" t="n">
         <v>265.8556410910593</v>
       </c>
-      <c r="X3" t="n">
-        <v>382.8566004433583</v>
-      </c>
-      <c r="Y3" t="n">
+      <c r="AL3" t="n">
+        <v>382.8566004433582</v>
+      </c>
+      <c r="AM3" t="n">
         <v>19.54214375698277</v>
       </c>
-      <c r="Z3" t="n">
+      <c r="AN3" t="n">
         <v>281.3605260728197</v>
       </c>
-      <c r="AA3" t="n">
+      <c r="AO3" t="n">
         <v>47.78193904311267</v>
       </c>
     </row>
@@ -747,81 +901,123 @@
         </is>
       </c>
       <c r="B4" t="n">
+        <v>101121.5096110575</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1398.95043196687</v>
+      </c>
+      <c r="D4" t="n">
+        <v>13119.47707968072</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4946.909167362483</v>
+      </c>
+      <c r="F4" t="n">
+        <v>475.9362426898699</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1376.876491532876</v>
+      </c>
+      <c r="H4" t="n">
+        <v>81.59013494508247</v>
+      </c>
+      <c r="I4" t="n">
+        <v>6323.785658895358</v>
+      </c>
+      <c r="J4" t="n">
+        <v>557.5263776349524</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1027.382494681306</v>
+      </c>
+      <c r="L4" t="n">
+        <v>55.23046715121213</v>
+      </c>
+      <c r="M4" t="n">
+        <v>870.5006003070322</v>
+      </c>
+      <c r="N4" t="n">
+        <v>138.3932627864787</v>
+      </c>
+      <c r="O4" t="n">
+        <v>337.581470170531</v>
+      </c>
+      <c r="P4" t="n">
         <v>39835.65461768988</v>
       </c>
-      <c r="C4" t="n">
+      <c r="Q4" t="n">
         <v>1642.562416926959</v>
       </c>
-      <c r="D4" t="n">
+      <c r="R4" t="n">
         <v>5888.771798129625</v>
       </c>
-      <c r="E4" t="n">
+      <c r="S4" t="n">
         <v>2214.43062076898</v>
       </c>
-      <c r="F4" t="n">
+      <c r="T4" t="n">
         <v>206.5063738952491</v>
       </c>
-      <c r="G4" t="n">
+      <c r="U4" t="n">
         <v>651.4409919283753</v>
       </c>
-      <c r="H4" t="n">
+      <c r="V4" t="n">
         <v>34.96197005383755</v>
       </c>
-      <c r="I4" t="n">
+      <c r="W4" t="n">
         <v>2865.871612697355</v>
       </c>
-      <c r="J4" t="n">
+      <c r="X4" t="n">
         <v>241.4683439490866</v>
       </c>
-      <c r="K4" t="n">
+      <c r="Y4" t="n">
         <v>384.7696365088916</v>
       </c>
-      <c r="L4" t="n">
+      <c r="Z4" t="n">
         <v>20.71681271646442</v>
       </c>
-      <c r="M4" t="n">
+      <c r="AA4" t="n">
         <v>288.9744933766121</v>
       </c>
-      <c r="N4" t="n">
+      <c r="AB4" t="n">
         <v>39.26688892702936</v>
       </c>
-      <c r="O4" t="n">
+      <c r="AC4" t="n">
         <v>33059.42705334981</v>
       </c>
-      <c r="P4" t="n">
+      <c r="AD4" t="n">
         <v>1710.777219034276</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="AE4" t="n">
         <v>5854.851126469145</v>
       </c>
-      <c r="R4" t="n">
+      <c r="AF4" t="n">
         <v>2330.013959716519</v>
       </c>
-      <c r="S4" t="n">
+      <c r="AG4" t="n">
         <v>213.6248492600263</v>
       </c>
-      <c r="T4" t="n">
+      <c r="AH4" t="n">
         <v>619.7484351617462</v>
       </c>
-      <c r="U4" t="n">
+      <c r="AI4" t="n">
         <v>30.44134379420773</v>
       </c>
-      <c r="V4" t="n">
+      <c r="AJ4" t="n">
         <v>2949.762394878265</v>
       </c>
-      <c r="W4" t="n">
+      <c r="AK4" t="n">
         <v>244.0661930542341</v>
       </c>
-      <c r="X4" t="n">
+      <c r="AL4" t="n">
         <v>366.0246009398963</v>
       </c>
-      <c r="Y4" t="n">
+      <c r="AM4" t="n">
         <v>17.43523994079843</v>
       </c>
-      <c r="Z4" t="n">
+      <c r="AN4" t="n">
         <v>268.7016179673131</v>
       </c>
-      <c r="AA4" t="n">
+      <c r="AO4" t="n">
         <v>42.72054323117423</v>
       </c>
     </row>
@@ -832,81 +1028,123 @@
         </is>
       </c>
       <c r="B5" t="n">
+        <v>101185.7202436983</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1520.66364081299</v>
+      </c>
+      <c r="D5" t="n">
+        <v>13218.74603481593</v>
+      </c>
+      <c r="E5" t="n">
+        <v>5069.685588293553</v>
+      </c>
+      <c r="F5" t="n">
+        <v>504.1076336743182</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1666.726257570293</v>
+      </c>
+      <c r="H5" t="n">
+        <v>93.68891676609157</v>
+      </c>
+      <c r="I5" t="n">
+        <v>6736.411845863846</v>
+      </c>
+      <c r="J5" t="n">
+        <v>597.7965504404096</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1051.554767565639</v>
+      </c>
+      <c r="L5" t="n">
+        <v>66.67264014296778</v>
+      </c>
+      <c r="M5" t="n">
+        <v>864.0240932544485</v>
+      </c>
+      <c r="N5" t="n">
+        <v>162.0473069603744</v>
+      </c>
+      <c r="O5" t="n">
+        <v>376.9914152822696</v>
+      </c>
+      <c r="P5" t="n">
         <v>36329.3198039069</v>
       </c>
-      <c r="C5" t="n">
+      <c r="Q5" t="n">
         <v>1796.3453528688</v>
       </c>
-      <c r="D5" t="n">
+      <c r="R5" t="n">
         <v>5485.629574808951</v>
       </c>
-      <c r="E5" t="n">
+      <c r="S5" t="n">
         <v>2253.566197583306</v>
       </c>
-      <c r="F5" t="n">
+      <c r="T5" t="n">
         <v>214.0807679957353</v>
       </c>
-      <c r="G5" t="n">
+      <c r="U5" t="n">
         <v>831.1872437403199</v>
       </c>
-      <c r="H5" t="n">
+      <c r="V5" t="n">
         <v>41.92023953273372</v>
       </c>
-      <c r="I5" t="n">
+      <c r="W5" t="n">
         <v>3084.753441323626</v>
       </c>
-      <c r="J5" t="n">
+      <c r="X5" t="n">
         <v>256.001007528469</v>
       </c>
-      <c r="K5" t="n">
+      <c r="Y5" t="n">
         <v>361.8716943300348</v>
       </c>
-      <c r="L5" t="n">
+      <c r="Z5" t="n">
         <v>22.9985057976689</v>
       </c>
-      <c r="M5" t="n">
+      <c r="AA5" t="n">
         <v>260.5669865292919</v>
       </c>
-      <c r="N5" t="n">
+      <c r="AB5" t="n">
         <v>39.72274921270161</v>
       </c>
-      <c r="O5" t="n">
+      <c r="AC5" t="n">
         <v>35826.4890328753</v>
       </c>
-      <c r="P5" t="n">
+      <c r="AD5" t="n">
         <v>1873.92649046366</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="AE5" t="n">
         <v>6339.066088984951</v>
       </c>
-      <c r="R5" t="n">
+      <c r="AF5" t="n">
         <v>2402.213546170371</v>
       </c>
-      <c r="S5" t="n">
+      <c r="AG5" t="n">
         <v>231.0500634971331</v>
       </c>
-      <c r="T5" t="n">
+      <c r="AH5" t="n">
         <v>679.3546493931528</v>
       </c>
-      <c r="U5" t="n">
+      <c r="AI5" t="n">
         <v>34.26146077844262</v>
       </c>
-      <c r="V5" t="n">
+      <c r="AJ5" t="n">
         <v>3081.568195563524</v>
       </c>
-      <c r="W5" t="n">
+      <c r="AK5" t="n">
         <v>265.3115242755757</v>
       </c>
-      <c r="X5" t="n">
+      <c r="AL5" t="n">
         <v>404.7662379128714</v>
       </c>
-      <c r="Y5" t="n">
+      <c r="AM5" t="n">
         <v>21.82375188926511</v>
       </c>
-      <c r="Z5" t="n">
+      <c r="AN5" t="n">
         <v>291.1439333807644</v>
       </c>
-      <c r="AA5" t="n">
+      <c r="AO5" t="n">
         <v>52.40385255022856</v>
       </c>
     </row>
@@ -917,81 +1155,123 @@
         </is>
       </c>
       <c r="B6" t="n">
+        <v>101817.8456814822</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1500.196284838452</v>
+      </c>
+      <c r="D6" t="n">
+        <v>14440.29166203201</v>
+      </c>
+      <c r="E6" t="n">
+        <v>5351.927120986315</v>
+      </c>
+      <c r="F6" t="n">
+        <v>517.1948958360886</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1691.404988595376</v>
+      </c>
+      <c r="H6" t="n">
+        <v>95.18758333784231</v>
+      </c>
+      <c r="I6" t="n">
+        <v>7043.33210958169</v>
+      </c>
+      <c r="J6" t="n">
+        <v>612.3824791739308</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1050.626633843435</v>
+      </c>
+      <c r="L6" t="n">
+        <v>65.71433311063242</v>
+      </c>
+      <c r="M6" t="n">
+        <v>864.2895015736029</v>
+      </c>
+      <c r="N6" t="n">
+        <v>158.4757740522624</v>
+      </c>
+      <c r="O6" t="n">
+        <v>371.9128461748793</v>
+      </c>
+      <c r="P6" t="n">
         <v>38364.30976201847</v>
       </c>
-      <c r="C6" t="n">
+      <c r="Q6" t="n">
         <v>1813.472520353595</v>
       </c>
-      <c r="D6" t="n">
+      <c r="R6" t="n">
         <v>6443.928726638457</v>
       </c>
-      <c r="E6" t="n">
+      <c r="S6" t="n">
         <v>2354.562312141525</v>
       </c>
-      <c r="F6" t="n">
+      <c r="T6" t="n">
         <v>223.5256608571924</v>
       </c>
-      <c r="G6" t="n">
+      <c r="U6" t="n">
         <v>841.4474052927986</v>
       </c>
-      <c r="H6" t="n">
+      <c r="V6" t="n">
         <v>42.20616749958173</v>
       </c>
-      <c r="I6" t="n">
+      <c r="W6" t="n">
         <v>3196.009717434323</v>
       </c>
-      <c r="J6" t="n">
+      <c r="X6" t="n">
         <v>265.7318283567741</v>
       </c>
-      <c r="K6" t="n">
+      <c r="Y6" t="n">
         <v>387.1249594865291</v>
       </c>
-      <c r="L6" t="n">
+      <c r="Z6" t="n">
         <v>23.39365086153757</v>
       </c>
-      <c r="M6" t="n">
+      <c r="AA6" t="n">
         <v>276.3745637222472</v>
       </c>
-      <c r="N6" t="n">
+      <c r="AB6" t="n">
         <v>41.63703451013856</v>
       </c>
-      <c r="O6" t="n">
+      <c r="AC6" t="n">
         <v>32315.64799448937</v>
       </c>
-      <c r="P6" t="n">
+      <c r="AD6" t="n">
         <v>1895.49159348734</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="AE6" t="n">
         <v>6329.355380213569</v>
       </c>
-      <c r="R6" t="n">
+      <c r="AF6" t="n">
         <v>2522.849394956393</v>
       </c>
-      <c r="S6" t="n">
+      <c r="AG6" t="n">
         <v>232.5703907408471</v>
       </c>
-      <c r="T6" t="n">
+      <c r="AH6" t="n">
         <v>683.3895994405326</v>
       </c>
-      <c r="U6" t="n">
+      <c r="AI6" t="n">
         <v>34.39571636840808</v>
       </c>
-      <c r="V6" t="n">
+      <c r="AJ6" t="n">
         <v>3206.238994396926</v>
       </c>
-      <c r="W6" t="n">
+      <c r="AK6" t="n">
         <v>266.9661071092552</v>
       </c>
-      <c r="X6" t="n">
+      <c r="AL6" t="n">
         <v>365.9224841371235</v>
       </c>
-      <c r="Y6" t="n">
+      <c r="AM6" t="n">
         <v>19.42781126609105</v>
       </c>
-      <c r="Z6" t="n">
+      <c r="AN6" t="n">
         <v>257.7601949884595</v>
       </c>
-      <c r="AA6" t="n">
+      <c r="AO6" t="n">
         <v>47.46906644811116</v>
       </c>
     </row>
@@ -1002,81 +1282,123 @@
         </is>
       </c>
       <c r="B7" t="n">
+        <v>103026.1195968547</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1512.676633769854</v>
+      </c>
+      <c r="D7" t="n">
+        <v>13977.52106333893</v>
+      </c>
+      <c r="E7" t="n">
+        <v>5399.3396824331</v>
+      </c>
+      <c r="F7" t="n">
+        <v>530.3050920113063</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1697.329065606786</v>
+      </c>
+      <c r="H7" t="n">
+        <v>99.89499369977753</v>
+      </c>
+      <c r="I7" t="n">
+        <v>7096.668748039887</v>
+      </c>
+      <c r="J7" t="n">
+        <v>630.2000857110838</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1088.759401937111</v>
+      </c>
+      <c r="L7" t="n">
+        <v>66.92139647224181</v>
+      </c>
+      <c r="M7" t="n">
+        <v>885.0464636511241</v>
+      </c>
+      <c r="N7" t="n">
+        <v>157.6955641123495</v>
+      </c>
+      <c r="O7" t="n">
+        <v>367.3364808916407</v>
+      </c>
+      <c r="P7" t="n">
         <v>35727.34822351123</v>
       </c>
-      <c r="C7" t="n">
+      <c r="Q7" t="n">
         <v>1824.941744244175</v>
       </c>
-      <c r="D7" t="n">
+      <c r="R7" t="n">
         <v>5778.054733501265</v>
       </c>
-      <c r="E7" t="n">
+      <c r="S7" t="n">
         <v>2374.034468055822</v>
       </c>
-      <c r="F7" t="n">
+      <c r="T7" t="n">
         <v>224.3303883474233</v>
       </c>
-      <c r="G7" t="n">
+      <c r="U7" t="n">
         <v>862.4096956328447</v>
       </c>
-      <c r="H7" t="n">
+      <c r="V7" t="n">
         <v>44.17597803273693</v>
       </c>
-      <c r="I7" t="n">
+      <c r="W7" t="n">
         <v>3236.444163688667</v>
       </c>
-      <c r="J7" t="n">
+      <c r="X7" t="n">
         <v>268.5063663801603</v>
       </c>
-      <c r="K7" t="n">
+      <c r="Y7" t="n">
         <v>373.9988628839857</v>
       </c>
-      <c r="L7" t="n">
+      <c r="Z7" t="n">
         <v>22.42705974676062</v>
       </c>
-      <c r="M7" t="n">
+      <c r="AA7" t="n">
         <v>266.3084704183372</v>
       </c>
-      <c r="N7" t="n">
+      <c r="AB7" t="n">
         <v>39.84229381419119</v>
       </c>
-      <c r="O7" t="n">
+      <c r="AC7" t="n">
         <v>35631.23939376771</v>
       </c>
-      <c r="P7" t="n">
+      <c r="AD7" t="n">
         <v>1889.975864980121</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="AE7" t="n">
         <v>6538.871685802329</v>
       </c>
-      <c r="R7" t="n">
+      <c r="AF7" t="n">
         <v>2553.280571057361</v>
       </c>
-      <c r="S7" t="n">
+      <c r="AG7" t="n">
         <v>244.9416110812896</v>
       </c>
-      <c r="T7" t="n">
+      <c r="AH7" t="n">
         <v>685.0519844463673</v>
       </c>
-      <c r="U7" t="n">
+      <c r="AI7" t="n">
         <v>37.24662424277886</v>
       </c>
-      <c r="V7" t="n">
+      <c r="AJ7" t="n">
         <v>3238.332555503728</v>
       </c>
-      <c r="W7" t="n">
+      <c r="AK7" t="n">
         <v>282.1882353240684</v>
       </c>
-      <c r="X7" t="n">
+      <c r="AL7" t="n">
         <v>404.2059888197002</v>
       </c>
-      <c r="Y7" t="n">
+      <c r="AM7" t="n">
         <v>20.576745637376</v>
       </c>
-      <c r="Z7" t="n">
+      <c r="AN7" t="n">
         <v>290.8971981268087</v>
       </c>
-      <c r="AA7" t="n">
+      <c r="AO7" t="n">
         <v>49.26548383392851</v>
       </c>
     </row>
@@ -1087,81 +1409,123 @@
         </is>
       </c>
       <c r="B8" t="n">
+        <v>101255.0626428813</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1433.525955729778</v>
+      </c>
+      <c r="D8" t="n">
+        <v>13549.89311698302</v>
+      </c>
+      <c r="E8" t="n">
+        <v>5136.762612015043</v>
+      </c>
+      <c r="F8" t="n">
+        <v>503.8214438327456</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1636.657815472032</v>
+      </c>
+      <c r="H8" t="n">
+        <v>93.18354079304683</v>
+      </c>
+      <c r="I8" t="n">
+        <v>6773.420427487074</v>
+      </c>
+      <c r="J8" t="n">
+        <v>597.0049846257925</v>
+      </c>
+      <c r="K8" t="n">
+        <v>1071.279365085949</v>
+      </c>
+      <c r="L8" t="n">
+        <v>65.23061150802504</v>
+      </c>
+      <c r="M8" t="n">
+        <v>866.4969320327705</v>
+      </c>
+      <c r="N8" t="n">
+        <v>156.1518324390342</v>
+      </c>
+      <c r="O8" t="n">
+        <v>352.9793963874367</v>
+      </c>
+      <c r="P8" t="n">
         <v>34951.32028616372</v>
       </c>
-      <c r="C8" t="n">
+      <c r="Q8" t="n">
         <v>1751.151805984811</v>
       </c>
-      <c r="D8" t="n">
+      <c r="R8" t="n">
         <v>5539.375957080137</v>
       </c>
-      <c r="E8" t="n">
+      <c r="S8" t="n">
         <v>2214.672902506505</v>
       </c>
-      <c r="F8" t="n">
+      <c r="T8" t="n">
         <v>211.3902208503606</v>
       </c>
-      <c r="G8" t="n">
+      <c r="U8" t="n">
         <v>840.4830441363794</v>
       </c>
-      <c r="H8" t="n">
+      <c r="V8" t="n">
         <v>42.23366861559504</v>
       </c>
-      <c r="I8" t="n">
+      <c r="W8" t="n">
         <v>3055.155946642884</v>
       </c>
-      <c r="J8" t="n">
+      <c r="X8" t="n">
         <v>253.6238894659556</v>
       </c>
-      <c r="K8" t="n">
+      <c r="Y8" t="n">
         <v>363.8326167412018</v>
       </c>
-      <c r="L8" t="n">
+      <c r="Z8" t="n">
         <v>21.65071469694586</v>
       </c>
-      <c r="M8" t="n">
+      <c r="AA8" t="n">
         <v>255.69757874504</v>
       </c>
-      <c r="N8" t="n">
+      <c r="AB8" t="n">
         <v>37.9413581141843</v>
       </c>
-      <c r="O8" t="n">
+      <c r="AC8" t="n">
         <v>36022.98809504891</v>
       </c>
-      <c r="P8" t="n">
+      <c r="AD8" t="n">
         <v>1771.447233404109</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="AE8" t="n">
         <v>6460.413959497083</v>
       </c>
-      <c r="R8" t="n">
+      <c r="AF8" t="n">
         <v>2495.709445324508</v>
       </c>
-      <c r="S8" t="n">
+      <c r="AG8" t="n">
         <v>238.0490047412358</v>
       </c>
-      <c r="T8" t="n">
+      <c r="AH8" t="n">
         <v>658.3429792237313</v>
       </c>
-      <c r="U8" t="n">
+      <c r="AI8" t="n">
         <v>35.26213437837964</v>
       </c>
-      <c r="V8" t="n">
+      <c r="AJ8" t="n">
         <v>3154.052424548239</v>
       </c>
-      <c r="W8" t="n">
+      <c r="AK8" t="n">
         <v>273.3111391196155</v>
       </c>
-      <c r="X8" t="n">
+      <c r="AL8" t="n">
         <v>413.4399324186161</v>
       </c>
-      <c r="Y8" t="n">
+      <c r="AM8" t="n">
         <v>20.2577579778538</v>
       </c>
-      <c r="Z8" t="n">
+      <c r="AN8" t="n">
         <v>300.2766371495229</v>
       </c>
-      <c r="AA8" t="n">
+      <c r="AO8" t="n">
         <v>51.06827590680861</v>
       </c>
     </row>
@@ -1172,81 +1536,123 @@
         </is>
       </c>
       <c r="B9" t="n">
+        <v>99966.58687170477</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1473.071932814785</v>
+      </c>
+      <c r="D9" t="n">
+        <v>13116.43486990435</v>
+      </c>
+      <c r="E9" t="n">
+        <v>5004.499265120869</v>
+      </c>
+      <c r="F9" t="n">
+        <v>502.8096848950382</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1551.156425887884</v>
+      </c>
+      <c r="H9" t="n">
+        <v>92.68616584188898</v>
+      </c>
+      <c r="I9" t="n">
+        <v>6555.655691008753</v>
+      </c>
+      <c r="J9" t="n">
+        <v>595.4958507369272</v>
+      </c>
+      <c r="K9" t="n">
+        <v>1063.824998958821</v>
+      </c>
+      <c r="L9" t="n">
+        <v>62.00944661818266</v>
+      </c>
+      <c r="M9" t="n">
+        <v>855.0215130929806</v>
+      </c>
+      <c r="N9" t="n">
+        <v>169.212898593574</v>
+      </c>
+      <c r="O9" t="n">
+        <v>368.5245351790625</v>
+      </c>
+      <c r="P9" t="n">
         <v>31712.65601471566</v>
       </c>
-      <c r="C9" t="n">
+      <c r="Q9" t="n">
         <v>1697.513342961181</v>
       </c>
-      <c r="D9" t="n">
+      <c r="R9" t="n">
         <v>4728.006377961241</v>
       </c>
-      <c r="E9" t="n">
+      <c r="S9" t="n">
         <v>1952.333528717393</v>
       </c>
-      <c r="F9" t="n">
+      <c r="T9" t="n">
         <v>192.5132950778745</v>
       </c>
-      <c r="G9" t="n">
+      <c r="U9" t="n">
         <v>704.3459205458515</v>
       </c>
-      <c r="H9" t="n">
+      <c r="V9" t="n">
         <v>36.80827451024174</v>
       </c>
-      <c r="I9" t="n">
+      <c r="W9" t="n">
         <v>2656.679449263244</v>
       </c>
-      <c r="J9" t="n">
+      <c r="X9" t="n">
         <v>229.3215695881162</v>
       </c>
-      <c r="K9" t="n">
+      <c r="Y9" t="n">
         <v>331.0493211637479</v>
       </c>
-      <c r="L9" t="n">
+      <c r="Z9" t="n">
         <v>18.82247802464963</v>
       </c>
-      <c r="M9" t="n">
+      <c r="AA9" t="n">
         <v>228.5377516086306</v>
       </c>
-      <c r="N9" t="n">
+      <c r="AB9" t="n">
         <v>38.90880828022765</v>
       </c>
-      <c r="O9" t="n">
+      <c r="AC9" t="n">
         <v>38629.15028659082</v>
       </c>
-      <c r="P9" t="n">
+      <c r="AD9" t="n">
         <v>1906.544449689495</v>
       </c>
-      <c r="Q9" t="n">
+      <c r="AE9" t="n">
         <v>7057.538681514773</v>
       </c>
-      <c r="R9" t="n">
+      <c r="AF9" t="n">
         <v>2625.852751651979</v>
       </c>
-      <c r="S9" t="n">
+      <c r="AG9" t="n">
         <v>250.3188464636979</v>
       </c>
-      <c r="T9" t="n">
+      <c r="AH9" t="n">
         <v>700.7098024968385</v>
       </c>
-      <c r="U9" t="n">
+      <c r="AI9" t="n">
         <v>37.74508253750755</v>
       </c>
-      <c r="V9" t="n">
+      <c r="AJ9" t="n">
         <v>3326.562554148817</v>
       </c>
-      <c r="W9" t="n">
+      <c r="AK9" t="n">
         <v>288.0639290012055</v>
       </c>
-      <c r="X9" t="n">
+      <c r="AL9" t="n">
         <v>433.0815423552864</v>
       </c>
-      <c r="Y9" t="n">
+      <c r="AM9" t="n">
         <v>19.99893606800926</v>
       </c>
-      <c r="Z9" t="n">
+      <c r="AN9" t="n">
         <v>313.2265431193254</v>
       </c>
-      <c r="AA9" t="n">
+      <c r="AO9" t="n">
         <v>55.35588011076818</v>
       </c>
     </row>
@@ -1257,81 +1663,123 @@
         </is>
       </c>
       <c r="B10" t="n">
+        <v>104268.4507363632</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1531.367821424719</v>
+      </c>
+      <c r="D10" t="n">
+        <v>14349.21324761732</v>
+      </c>
+      <c r="E10" t="n">
+        <v>5147.900065699176</v>
+      </c>
+      <c r="F10" t="n">
+        <v>482.3378628267972</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1396.791408818709</v>
+      </c>
+      <c r="H10" t="n">
+        <v>82.25832886278064</v>
+      </c>
+      <c r="I10" t="n">
+        <v>6544.691474517885</v>
+      </c>
+      <c r="J10" t="n">
+        <v>564.5961916895779</v>
+      </c>
+      <c r="K10" t="n">
+        <v>1033.482388513996</v>
+      </c>
+      <c r="L10" t="n">
+        <v>56.6623185117708</v>
+      </c>
+      <c r="M10" t="n">
+        <v>859.7566105038591</v>
+      </c>
+      <c r="N10" t="n">
+        <v>145.4461546644024</v>
+      </c>
+      <c r="O10" t="n">
+        <v>363.6703866776008</v>
+      </c>
+      <c r="P10" t="n">
         <v>34599.30578078904</v>
       </c>
-      <c r="C10" t="n">
+      <c r="Q10" t="n">
         <v>1813.768055238299</v>
       </c>
-      <c r="D10" t="n">
+      <c r="R10" t="n">
         <v>5636.938385052741</v>
       </c>
-      <c r="E10" t="n">
+      <c r="S10" t="n">
         <v>2165.221969408223</v>
       </c>
-      <c r="F10" t="n">
+      <c r="T10" t="n">
         <v>198.1199025707598</v>
       </c>
-      <c r="G10" t="n">
+      <c r="U10" t="n">
         <v>664.0143623256224</v>
       </c>
-      <c r="H10" t="n">
+      <c r="V10" t="n">
         <v>35.03201147873428</v>
       </c>
-      <c r="I10" t="n">
+      <c r="W10" t="n">
         <v>2829.236331733845</v>
       </c>
-      <c r="J10" t="n">
+      <c r="X10" t="n">
         <v>233.1519140494941</v>
       </c>
-      <c r="K10" t="n">
+      <c r="Y10" t="n">
         <v>348.0469324585746</v>
       </c>
-      <c r="L10" t="n">
+      <c r="Z10" t="n">
         <v>18.02493926423912</v>
       </c>
-      <c r="M10" t="n">
+      <c r="AA10" t="n">
         <v>243.1907355472126</v>
       </c>
-      <c r="N10" t="n">
+      <c r="AB10" t="n">
         <v>36.78198422600281</v>
       </c>
-      <c r="O10" t="n">
+      <c r="AC10" t="n">
         <v>38013.70916507281</v>
       </c>
-      <c r="P10" t="n">
+      <c r="AD10" t="n">
         <v>1934.21398782214</v>
       </c>
-      <c r="Q10" t="n">
+      <c r="AE10" t="n">
         <v>7104.278146511607</v>
       </c>
-      <c r="R10" t="n">
+      <c r="AF10" t="n">
         <v>2530.029499378603</v>
       </c>
-      <c r="S10" t="n">
+      <c r="AG10" t="n">
         <v>228.0049846634972</v>
       </c>
-      <c r="T10" t="n">
+      <c r="AH10" t="n">
         <v>607.239011985018</v>
       </c>
-      <c r="U10" t="n">
+      <c r="AI10" t="n">
         <v>30.51344935987909</v>
       </c>
-      <c r="V10" t="n">
+      <c r="AJ10" t="n">
         <v>3137.26851136362</v>
       </c>
-      <c r="W10" t="n">
+      <c r="AK10" t="n">
         <v>258.5184340233763</v>
       </c>
-      <c r="X10" t="n">
+      <c r="AL10" t="n">
         <v>397.0339840138156</v>
       </c>
-      <c r="Y10" t="n">
+      <c r="AM10" t="n">
         <v>19.09787495587503</v>
       </c>
-      <c r="Z10" t="n">
+      <c r="AN10" t="n">
         <v>294.1851427522167</v>
       </c>
-      <c r="AA10" t="n">
+      <c r="AO10" t="n">
         <v>46.66148726448649</v>
       </c>
     </row>
@@ -1342,81 +1790,123 @@
         </is>
       </c>
       <c r="B11" t="n">
+        <v>101318.4385125295</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1501.42491293612</v>
+      </c>
+      <c r="D11" t="n">
+        <v>13365.16966307162</v>
+      </c>
+      <c r="E11" t="n">
+        <v>4916.291709451431</v>
+      </c>
+      <c r="F11" t="n">
+        <v>486.7779696286011</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1542.828242279128</v>
+      </c>
+      <c r="H11" t="n">
+        <v>87.19699288047084</v>
+      </c>
+      <c r="I11" t="n">
+        <v>6459.119951730558</v>
+      </c>
+      <c r="J11" t="n">
+        <v>573.9749625090718</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1020.74291875804</v>
+      </c>
+      <c r="L11" t="n">
+        <v>61.52101714583087</v>
+      </c>
+      <c r="M11" t="n">
+        <v>851.5097248061735</v>
+      </c>
+      <c r="N11" t="n">
+        <v>152.9816412607639</v>
+      </c>
+      <c r="O11" t="n">
+        <v>374.3856567947199</v>
+      </c>
+      <c r="P11" t="n">
         <v>33556.87371432573</v>
       </c>
-      <c r="C11" t="n">
+      <c r="Q11" t="n">
         <v>1814.323322454931</v>
       </c>
-      <c r="D11" t="n">
+      <c r="R11" t="n">
         <v>5260.150160628757</v>
       </c>
-      <c r="E11" t="n">
+      <c r="S11" t="n">
         <v>2196.798965504275</v>
       </c>
-      <c r="F11" t="n">
+      <c r="T11" t="n">
         <v>209.5475429531017</v>
       </c>
-      <c r="G11" t="n">
+      <c r="U11" t="n">
         <v>769.2388941444563</v>
       </c>
-      <c r="H11" t="n">
+      <c r="V11" t="n">
         <v>38.5938364196981</v>
       </c>
-      <c r="I11" t="n">
+      <c r="W11" t="n">
         <v>2966.037859648732</v>
       </c>
-      <c r="J11" t="n">
+      <c r="X11" t="n">
         <v>248.1413793727997</v>
       </c>
-      <c r="K11" t="n">
+      <c r="Y11" t="n">
         <v>338.6410023512584</v>
       </c>
-      <c r="L11" t="n">
+      <c r="Z11" t="n">
         <v>20.44505142322577</v>
       </c>
-      <c r="M11" t="n">
+      <c r="AA11" t="n">
         <v>236.9468140317591</v>
       </c>
-      <c r="N11" t="n">
+      <c r="AB11" t="n">
         <v>37.53058492236872</v>
       </c>
-      <c r="O11" t="n">
+      <c r="AC11" t="n">
         <v>37795.27953249563</v>
       </c>
-      <c r="P11" t="n">
+      <c r="AD11" t="n">
         <v>1902.70474997408</v>
       </c>
-      <c r="Q11" t="n">
+      <c r="AE11" t="n">
         <v>6709.321416079494</v>
       </c>
-      <c r="R11" t="n">
+      <c r="AF11" t="n">
         <v>2320.804939557562</v>
       </c>
-      <c r="S11" t="n">
+      <c r="AG11" t="n">
         <v>221.8202145568863</v>
       </c>
-      <c r="T11" t="n">
+      <c r="AH11" t="n">
         <v>640.4599988154947</v>
       </c>
-      <c r="U11" t="n">
+      <c r="AI11" t="n">
         <v>31.51960780515648</v>
       </c>
-      <c r="V11" t="n">
+      <c r="AJ11" t="n">
         <v>2961.264938373056</v>
       </c>
-      <c r="W11" t="n">
+      <c r="AK11" t="n">
         <v>253.3398223620428</v>
       </c>
-      <c r="X11" t="n">
+      <c r="AL11" t="n">
         <v>398.2331604895535</v>
       </c>
-      <c r="Y11" t="n">
+      <c r="AM11" t="n">
         <v>20.11182949080873</v>
       </c>
-      <c r="Z11" t="n">
+      <c r="AN11" t="n">
         <v>300.9267137088569</v>
       </c>
-      <c r="AA11" t="n">
+      <c r="AO11" t="n">
         <v>48.10667988009593</v>
       </c>
     </row>
@@ -1427,81 +1917,123 @@
         </is>
       </c>
       <c r="B12" t="n">
+        <v>101504.2676026991</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1414.563064016289</v>
+      </c>
+      <c r="D12" t="n">
+        <v>13538.94141851859</v>
+      </c>
+      <c r="E12" t="n">
+        <v>5380.298359490952</v>
+      </c>
+      <c r="F12" t="n">
+        <v>516.8162165985245</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1636.26492091476</v>
+      </c>
+      <c r="H12" t="n">
+        <v>95.81032931745709</v>
+      </c>
+      <c r="I12" t="n">
+        <v>7016.563280405711</v>
+      </c>
+      <c r="J12" t="n">
+        <v>612.6265459159816</v>
+      </c>
+      <c r="K12" t="n">
+        <v>1023.994182417704</v>
+      </c>
+      <c r="L12" t="n">
+        <v>61.69265540872984</v>
+      </c>
+      <c r="M12" t="n">
+        <v>831.952186859352</v>
+      </c>
+      <c r="N12" t="n">
+        <v>148.2021841626865</v>
+      </c>
+      <c r="O12" t="n">
+        <v>349.2217523827069</v>
+      </c>
+      <c r="P12" t="n">
         <v>31924.77795037885</v>
       </c>
-      <c r="C12" t="n">
+      <c r="Q12" t="n">
         <v>1709.226529569799</v>
       </c>
-      <c r="D12" t="n">
+      <c r="R12" t="n">
         <v>4951.300566856832</v>
       </c>
-      <c r="E12" t="n">
+      <c r="S12" t="n">
         <v>1989.14131314416</v>
       </c>
-      <c r="F12" t="n">
+      <c r="T12" t="n">
         <v>188.511910952724</v>
       </c>
-      <c r="G12" t="n">
+      <c r="U12" t="n">
         <v>667.0945804989935</v>
       </c>
-      <c r="H12" t="n">
+      <c r="V12" t="n">
         <v>34.36742642369819</v>
       </c>
-      <c r="I12" t="n">
+      <c r="W12" t="n">
         <v>2656.235893643154</v>
       </c>
-      <c r="J12" t="n">
+      <c r="X12" t="n">
         <v>222.8793373764222</v>
       </c>
-      <c r="K12" t="n">
+      <c r="Y12" t="n">
         <v>323.1572713646102</v>
       </c>
-      <c r="L12" t="n">
+      <c r="Z12" t="n">
         <v>19.40959774174423</v>
       </c>
-      <c r="M12" t="n">
+      <c r="AA12" t="n">
         <v>222.1603472937751</v>
       </c>
-      <c r="N12" t="n">
+      <c r="AB12" t="n">
         <v>33.83238760043948</v>
       </c>
-      <c r="O12" t="n">
+      <c r="AC12" t="n">
         <v>37177.20980042957</v>
       </c>
-      <c r="P12" t="n">
+      <c r="AD12" t="n">
         <v>1882.029628096796</v>
       </c>
-      <c r="Q12" t="n">
+      <c r="AE12" t="n">
         <v>6997.97720980198</v>
       </c>
-      <c r="R12" t="n">
+      <c r="AF12" t="n">
         <v>2951.406684730563</v>
       </c>
-      <c r="S12" t="n">
+      <c r="AG12" t="n">
         <v>272.2086915090495</v>
       </c>
-      <c r="T12" t="n">
+      <c r="AH12" t="n">
         <v>839.1136476804604</v>
       </c>
-      <c r="U12" t="n">
+      <c r="AI12" t="n">
         <v>44.37879488398616</v>
       </c>
-      <c r="V12" t="n">
+      <c r="AJ12" t="n">
         <v>3790.520332411023</v>
       </c>
-      <c r="W12" t="n">
+      <c r="AK12" t="n">
         <v>316.5874863930357</v>
       </c>
-      <c r="X12" t="n">
+      <c r="AL12" t="n">
         <v>404.8806935345627</v>
       </c>
-      <c r="Y12" t="n">
+      <c r="AM12" t="n">
         <v>21.74811024745186</v>
       </c>
-      <c r="Z12" t="n">
+      <c r="AN12" t="n">
         <v>293.8804295773204</v>
       </c>
-      <c r="AA12" t="n">
+      <c r="AO12" t="n">
         <v>50.92385965164715</v>
       </c>
     </row>
@@ -1512,81 +2044,123 @@
         </is>
       </c>
       <c r="B13" t="n">
+        <v>101918.6079795883</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1445.188801727647</v>
+      </c>
+      <c r="D13" t="n">
+        <v>14213.40318142749</v>
+      </c>
+      <c r="E13" t="n">
+        <v>5076.284194743098</v>
+      </c>
+      <c r="F13" t="n">
+        <v>479.2623421385697</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1333.496865591414</v>
+      </c>
+      <c r="H13" t="n">
+        <v>79.46233176170961</v>
+      </c>
+      <c r="I13" t="n">
+        <v>6409.781060334512</v>
+      </c>
+      <c r="J13" t="n">
+        <v>558.7246739002793</v>
+      </c>
+      <c r="K13" t="n">
+        <v>1063.63077268115</v>
+      </c>
+      <c r="L13" t="n">
+        <v>59.22802320384861</v>
+      </c>
+      <c r="M13" t="n">
+        <v>872.5521391320598</v>
+      </c>
+      <c r="N13" t="n">
+        <v>152.7289038715696</v>
+      </c>
+      <c r="O13" t="n">
+        <v>349.5182139877469</v>
+      </c>
+      <c r="P13" t="n">
         <v>33400.81349215898</v>
       </c>
-      <c r="C13" t="n">
+      <c r="Q13" t="n">
         <v>1753.497097978196</v>
       </c>
-      <c r="D13" t="n">
+      <c r="R13" t="n">
         <v>5492.744281768415</v>
       </c>
-      <c r="E13" t="n">
+      <c r="S13" t="n">
         <v>2081.617532743563</v>
       </c>
-      <c r="F13" t="n">
+      <c r="T13" t="n">
         <v>191.1969619314859</v>
       </c>
-      <c r="G13" t="n">
+      <c r="U13" t="n">
         <v>609.0852414515706</v>
       </c>
-      <c r="H13" t="n">
+      <c r="V13" t="n">
         <v>32.26976470417866</v>
       </c>
-      <c r="I13" t="n">
+      <c r="W13" t="n">
         <v>2690.702774195134</v>
       </c>
-      <c r="J13" t="n">
+      <c r="X13" t="n">
         <v>223.4667266356646</v>
       </c>
-      <c r="K13" t="n">
+      <c r="Y13" t="n">
         <v>335.7716657760849</v>
       </c>
-      <c r="L13" t="n">
+      <c r="Z13" t="n">
         <v>18.17784094726269</v>
       </c>
-      <c r="M13" t="n">
+      <c r="AA13" t="n">
         <v>238.7297038298212</v>
       </c>
-      <c r="N13" t="n">
+      <c r="AB13" t="n">
         <v>37.66836162969642</v>
       </c>
-      <c r="O13" t="n">
+      <c r="AC13" t="n">
         <v>36883.66617384075</v>
       </c>
-      <c r="P13" t="n">
+      <c r="AD13" t="n">
         <v>1840.583584579148</v>
       </c>
-      <c r="Q13" t="n">
+      <c r="AE13" t="n">
         <v>7100.825748611669</v>
       </c>
-      <c r="R13" t="n">
+      <c r="AF13" t="n">
         <v>2564.479362394357</v>
       </c>
-      <c r="S13" t="n">
+      <c r="AG13" t="n">
         <v>232.6371150823617</v>
       </c>
-      <c r="T13" t="n">
+      <c r="AH13" t="n">
         <v>601.7674645570363</v>
       </c>
-      <c r="U13" t="n">
+      <c r="AI13" t="n">
         <v>31.38321765866515</v>
       </c>
-      <c r="V13" t="n">
+      <c r="AJ13" t="n">
         <v>3166.246826951393</v>
       </c>
-      <c r="W13" t="n">
+      <c r="AK13" t="n">
         <v>264.0203327410269</v>
       </c>
-      <c r="X13" t="n">
+      <c r="AL13" t="n">
         <v>421.6225187593739</v>
       </c>
-      <c r="Y13" t="n">
+      <c r="AM13" t="n">
         <v>18.9610097184604</v>
       </c>
-      <c r="Z13" t="n">
+      <c r="AN13" t="n">
         <v>313.0607988831151</v>
       </c>
-      <c r="AA13" t="n">
+      <c r="AO13" t="n">
         <v>49.10175908112218</v>
       </c>
     </row>
@@ -1597,81 +2171,123 @@
         </is>
       </c>
       <c r="B14" t="n">
+        <v>103973.4795058257</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1481.277698008819</v>
+      </c>
+      <c r="D14" t="n">
+        <v>14618.30311828344</v>
+      </c>
+      <c r="E14" t="n">
+        <v>5406.326763169487</v>
+      </c>
+      <c r="F14" t="n">
+        <v>523.4717731236101</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1578.103807316056</v>
+      </c>
+      <c r="H14" t="n">
+        <v>93.76180041691894</v>
+      </c>
+      <c r="I14" t="n">
+        <v>6984.430570485543</v>
+      </c>
+      <c r="J14" t="n">
+        <v>617.2335735405291</v>
+      </c>
+      <c r="K14" t="n">
+        <v>1069.887141654378</v>
+      </c>
+      <c r="L14" t="n">
+        <v>59.9106813107798</v>
+      </c>
+      <c r="M14" t="n">
+        <v>879.1403299300923</v>
+      </c>
+      <c r="N14" t="n">
+        <v>148.6640877132417</v>
+      </c>
+      <c r="O14" t="n">
+        <v>354.1441979270216</v>
+      </c>
+      <c r="P14" t="n">
         <v>32689.01741591886</v>
       </c>
-      <c r="C14" t="n">
+      <c r="Q14" t="n">
         <v>1701.174526645647</v>
       </c>
-      <c r="D14" t="n">
+      <c r="R14" t="n">
         <v>5112.88799434892</v>
       </c>
-      <c r="E14" t="n">
+      <c r="S14" t="n">
         <v>1964.282481062862</v>
       </c>
-      <c r="F14" t="n">
+      <c r="T14" t="n">
         <v>187.7923593051985</v>
       </c>
-      <c r="G14" t="n">
+      <c r="U14" t="n">
         <v>624.7304372284598</v>
       </c>
-      <c r="H14" t="n">
+      <c r="V14" t="n">
         <v>32.37312598259111</v>
       </c>
-      <c r="I14" t="n">
+      <c r="W14" t="n">
         <v>2589.012918291322</v>
       </c>
-      <c r="J14" t="n">
+      <c r="X14" t="n">
         <v>220.1654852877896</v>
       </c>
-      <c r="K14" t="n">
+      <c r="Y14" t="n">
         <v>337.2911964459875</v>
       </c>
-      <c r="L14" t="n">
+      <c r="Z14" t="n">
         <v>18.38693421152254</v>
       </c>
-      <c r="M14" t="n">
+      <c r="AA14" t="n">
         <v>233.117807080912</v>
       </c>
-      <c r="N14" t="n">
+      <c r="AB14" t="n">
         <v>34.21036933884186</v>
       </c>
-      <c r="O14" t="n">
+      <c r="AC14" t="n">
         <v>40668.16497309941</v>
       </c>
-      <c r="P14" t="n">
+      <c r="AD14" t="n">
         <v>1853.31725983307</v>
       </c>
-      <c r="Q14" t="n">
+      <c r="AE14" t="n">
         <v>7913.337624110826</v>
       </c>
-      <c r="R14" t="n">
+      <c r="AF14" t="n">
         <v>2996.468541485473</v>
       </c>
-      <c r="S14" t="n">
+      <c r="AG14" t="n">
         <v>282.3192247311213</v>
       </c>
-      <c r="T14" t="n">
+      <c r="AH14" t="n">
         <v>825.5512108868013</v>
       </c>
-      <c r="U14" t="n">
+      <c r="AI14" t="n">
         <v>43.97405884210976</v>
       </c>
-      <c r="V14" t="n">
+      <c r="AJ14" t="n">
         <v>3822.019752372274</v>
       </c>
-      <c r="W14" t="n">
+      <c r="AK14" t="n">
         <v>326.2932835732311</v>
       </c>
-      <c r="X14" t="n">
+      <c r="AL14" t="n">
         <v>443.1763366070703</v>
       </c>
-      <c r="Y14" t="n">
+      <c r="AM14" t="n">
         <v>21.16522445671716</v>
       </c>
-      <c r="Z14" t="n">
+      <c r="AN14" t="n">
         <v>325.5251420143118</v>
       </c>
-      <c r="AA14" t="n">
+      <c r="AO14" t="n">
         <v>52.36861314931601</v>
       </c>
     </row>
@@ -1682,81 +2298,123 @@
         </is>
       </c>
       <c r="B15" t="n">
+        <v>100493.3754723208</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1522.763705409455</v>
+      </c>
+      <c r="D15" t="n">
+        <v>13334.84129655099</v>
+      </c>
+      <c r="E15" t="n">
+        <v>5041.724871329062</v>
+      </c>
+      <c r="F15" t="n">
+        <v>489.5514501933911</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1545.380260301615</v>
+      </c>
+      <c r="H15" t="n">
+        <v>89.72928952969373</v>
+      </c>
+      <c r="I15" t="n">
+        <v>6587.105131630678</v>
+      </c>
+      <c r="J15" t="n">
+        <v>579.2807397230848</v>
+      </c>
+      <c r="K15" t="n">
+        <v>1055.312932747007</v>
+      </c>
+      <c r="L15" t="n">
+        <v>65.26381728604041</v>
+      </c>
+      <c r="M15" t="n">
+        <v>867.9193931312163</v>
+      </c>
+      <c r="N15" t="n">
+        <v>154.9027853706336</v>
+      </c>
+      <c r="O15" t="n">
+        <v>379.6420174970298</v>
+      </c>
+      <c r="P15" t="n">
         <v>34622.12060813731</v>
       </c>
-      <c r="C15" t="n">
+      <c r="Q15" t="n">
         <v>1798.640002538314</v>
       </c>
-      <c r="D15" t="n">
+      <c r="R15" t="n">
         <v>5211.75227434212</v>
       </c>
-      <c r="E15" t="n">
+      <c r="S15" t="n">
         <v>2058.586320347985</v>
       </c>
-      <c r="F15" t="n">
+      <c r="T15" t="n">
         <v>193.3570242230889</v>
       </c>
-      <c r="G15" t="n">
+      <c r="U15" t="n">
         <v>709.8461316887618</v>
       </c>
-      <c r="H15" t="n">
+      <c r="V15" t="n">
         <v>35.25963866816105</v>
       </c>
-      <c r="I15" t="n">
+      <c r="W15" t="n">
         <v>2768.432452036747</v>
       </c>
-      <c r="J15" t="n">
+      <c r="X15" t="n">
         <v>228.6166628912499</v>
       </c>
-      <c r="K15" t="n">
+      <c r="Y15" t="n">
         <v>348.2456417825973</v>
       </c>
-      <c r="L15" t="n">
+      <c r="Z15" t="n">
         <v>20.78726325078235</v>
       </c>
-      <c r="M15" t="n">
+      <c r="AA15" t="n">
         <v>249.0724970614975</v>
       </c>
-      <c r="N15" t="n">
+      <c r="AB15" t="n">
         <v>37.82702651580312</v>
       </c>
-      <c r="O15" t="n">
+      <c r="AC15" t="n">
         <v>35956.11748919122</v>
       </c>
-      <c r="P15" t="n">
+      <c r="AD15" t="n">
         <v>1914.32467951373</v>
       </c>
-      <c r="Q15" t="n">
+      <c r="AE15" t="n">
         <v>6648.11881062922</v>
       </c>
-      <c r="R15" t="n">
+      <c r="AF15" t="n">
         <v>2571.577495722455</v>
       </c>
-      <c r="S15" t="n">
+      <c r="AG15" t="n">
         <v>241.3841052808941</v>
       </c>
-      <c r="T15" t="n">
+      <c r="AH15" t="n">
         <v>692.7725020088776</v>
       </c>
-      <c r="U15" t="n">
+      <c r="AI15" t="n">
         <v>36.62463872834574</v>
       </c>
-      <c r="V15" t="n">
+      <c r="AJ15" t="n">
         <v>3264.349997731333</v>
       </c>
-      <c r="W15" t="n">
+      <c r="AK15" t="n">
         <v>278.0087440092399</v>
       </c>
-      <c r="X15" t="n">
+      <c r="AL15" t="n">
         <v>402.5917815805749</v>
       </c>
-      <c r="Y15" t="n">
+      <c r="AM15" t="n">
         <v>20.58818266223681</v>
       </c>
-      <c r="Z15" t="n">
+      <c r="AN15" t="n">
         <v>295.1599233991067</v>
       </c>
-      <c r="AA15" t="n">
+      <c r="AO15" t="n">
         <v>48.25928335638009</v>
       </c>
     </row>
@@ -1767,81 +2425,123 @@
         </is>
       </c>
       <c r="B16" t="n">
+        <v>100662.2842542938</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1497.058482150735</v>
+      </c>
+      <c r="D16" t="n">
+        <v>13604.15933127078</v>
+      </c>
+      <c r="E16" t="n">
+        <v>5068.021078168229</v>
+      </c>
+      <c r="F16" t="n">
+        <v>484.6040365457534</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1478.576078574107</v>
+      </c>
+      <c r="H16" t="n">
+        <v>84.6899034474618</v>
+      </c>
+      <c r="I16" t="n">
+        <v>6546.597156742336</v>
+      </c>
+      <c r="J16" t="n">
+        <v>569.2939399932152</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1049.80230181413</v>
+      </c>
+      <c r="L16" t="n">
+        <v>60.52273971881706</v>
+      </c>
+      <c r="M16" t="n">
+        <v>873.5803331957856</v>
+      </c>
+      <c r="N16" t="n">
+        <v>147.2136323395296</v>
+      </c>
+      <c r="O16" t="n">
+        <v>368.0552062990036</v>
+      </c>
+      <c r="P16" t="n">
         <v>30834.49821083745</v>
       </c>
-      <c r="C16" t="n">
+      <c r="Q16" t="n">
         <v>1824.955169983611</v>
       </c>
-      <c r="D16" t="n">
+      <c r="R16" t="n">
         <v>4808.138677226871</v>
       </c>
-      <c r="E16" t="n">
+      <c r="S16" t="n">
         <v>1966.247746387659</v>
       </c>
-      <c r="F16" t="n">
+      <c r="T16" t="n">
         <v>185.8928085102627</v>
       </c>
-      <c r="G16" t="n">
+      <c r="U16" t="n">
         <v>684.0892388843872</v>
       </c>
-      <c r="H16" t="n">
+      <c r="V16" t="n">
         <v>34.48313997859874</v>
       </c>
-      <c r="I16" t="n">
+      <c r="W16" t="n">
         <v>2650.336985272047</v>
       </c>
-      <c r="J16" t="n">
+      <c r="X16" t="n">
         <v>220.3759484888615</v>
       </c>
-      <c r="K16" t="n">
+      <c r="Y16" t="n">
         <v>316.4500301182314</v>
       </c>
-      <c r="L16" t="n">
+      <c r="Z16" t="n">
         <v>18.55154460157359</v>
       </c>
-      <c r="M16" t="n">
+      <c r="AA16" t="n">
         <v>224.1898755806921</v>
       </c>
-      <c r="N16" t="n">
+      <c r="AB16" t="n">
         <v>34.12680711643406</v>
       </c>
-      <c r="O16" t="n">
+      <c r="AC16" t="n">
         <v>39333.47810827673</v>
       </c>
-      <c r="P16" t="n">
+      <c r="AD16" t="n">
         <v>1950.234577710387</v>
       </c>
-      <c r="Q16" t="n">
+      <c r="AE16" t="n">
         <v>7275.18438381999</v>
       </c>
-      <c r="R16" t="n">
+      <c r="AF16" t="n">
         <v>2661.962250527356</v>
       </c>
-      <c r="S16" t="n">
+      <c r="AG16" t="n">
         <v>242.7975147658969</v>
       </c>
-      <c r="T16" t="n">
+      <c r="AH16" t="n">
         <v>662.3447190965047</v>
       </c>
-      <c r="U16" t="n">
+      <c r="AI16" t="n">
         <v>32.7655537530103</v>
       </c>
-      <c r="V16" t="n">
+      <c r="AJ16" t="n">
         <v>3324.306969623861</v>
       </c>
-      <c r="W16" t="n">
+      <c r="AK16" t="n">
         <v>275.5630685189072</v>
       </c>
-      <c r="X16" t="n">
+      <c r="AL16" t="n">
         <v>435.2114100255834</v>
       </c>
-      <c r="Y16" t="n">
+      <c r="AM16" t="n">
         <v>19.19037990539216</v>
       </c>
-      <c r="Z16" t="n">
+      <c r="AN16" t="n">
         <v>327.9275164545384</v>
       </c>
-      <c r="AA16" t="n">
+      <c r="AO16" t="n">
         <v>51.24997588561863</v>
       </c>
     </row>
@@ -1852,81 +2552,123 @@
         </is>
       </c>
       <c r="B17" t="n">
+        <v>103105.711464443</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1478.520317686502</v>
+      </c>
+      <c r="D17" t="n">
+        <v>14179.60914402903</v>
+      </c>
+      <c r="E17" t="n">
+        <v>5308.669397156812</v>
+      </c>
+      <c r="F17" t="n">
+        <v>500.997000334099</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1559.182741941554</v>
+      </c>
+      <c r="H17" t="n">
+        <v>90.72026591831778</v>
+      </c>
+      <c r="I17" t="n">
+        <v>6867.852139098365</v>
+      </c>
+      <c r="J17" t="n">
+        <v>591.7172662524168</v>
+      </c>
+      <c r="K17" t="n">
+        <v>1061.069164432501</v>
+      </c>
+      <c r="L17" t="n">
+        <v>56.66827877130893</v>
+      </c>
+      <c r="M17" t="n">
+        <v>870.5844529004797</v>
+      </c>
+      <c r="N17" t="n">
+        <v>154.5113764439112</v>
+      </c>
+      <c r="O17" t="n">
+        <v>358.5480470031791</v>
+      </c>
+      <c r="P17" t="n">
         <v>32197.91631945951</v>
       </c>
-      <c r="C17" t="n">
+      <c r="Q17" t="n">
         <v>1805.582730617899</v>
       </c>
-      <c r="D17" t="n">
+      <c r="R17" t="n">
         <v>5287.461061073574</v>
       </c>
-      <c r="E17" t="n">
+      <c r="S17" t="n">
         <v>2182.108513671355</v>
       </c>
-      <c r="F17" t="n">
+      <c r="T17" t="n">
         <v>200.337664868818</v>
       </c>
-      <c r="G17" t="n">
+      <c r="U17" t="n">
         <v>733.223326592201</v>
       </c>
-      <c r="H17" t="n">
+      <c r="V17" t="n">
         <v>37.13326301539426</v>
       </c>
-      <c r="I17" t="n">
+      <c r="W17" t="n">
         <v>2915.331840263556</v>
       </c>
-      <c r="J17" t="n">
+      <c r="X17" t="n">
         <v>237.4709278842122</v>
       </c>
-      <c r="K17" t="n">
+      <c r="Y17" t="n">
         <v>325.5494735320646</v>
       </c>
-      <c r="L17" t="n">
+      <c r="Z17" t="n">
         <v>17.62620049982698</v>
       </c>
-      <c r="M17" t="n">
+      <c r="AA17" t="n">
         <v>227.2553887637085</v>
       </c>
-      <c r="N17" t="n">
+      <c r="AB17" t="n">
         <v>36.11733105354341</v>
       </c>
-      <c r="O17" t="n">
+      <c r="AC17" t="n">
         <v>38227.21615555442</v>
       </c>
-      <c r="P17" t="n">
+      <c r="AD17" t="n">
         <v>1907.749988971838</v>
       </c>
-      <c r="Q17" t="n">
+      <c r="AE17" t="n">
         <v>7201.163201644224</v>
       </c>
-      <c r="R17" t="n">
+      <c r="AF17" t="n">
         <v>2671.698051368409</v>
       </c>
-      <c r="S17" t="n">
+      <c r="AG17" t="n">
         <v>245.2744887391809</v>
       </c>
-      <c r="T17" t="n">
+      <c r="AH17" t="n">
         <v>703.5289181469866</v>
       </c>
-      <c r="U17" t="n">
+      <c r="AI17" t="n">
         <v>36.12723154371011</v>
       </c>
-      <c r="V17" t="n">
+      <c r="AJ17" t="n">
         <v>3375.226969515396</v>
       </c>
-      <c r="W17" t="n">
+      <c r="AK17" t="n">
         <v>281.4017202828911</v>
       </c>
-      <c r="X17" t="n">
+      <c r="AL17" t="n">
         <v>411.1229662586708</v>
       </c>
-      <c r="Y17" t="n">
+      <c r="AM17" t="n">
         <v>18.45047282502311</v>
       </c>
-      <c r="Z17" t="n">
+      <c r="AN17" t="n">
         <v>308.5979099002224</v>
       </c>
-      <c r="AA17" t="n">
+      <c r="AO17" t="n">
         <v>47.84697068360161</v>
       </c>
     </row>
@@ -1937,81 +2679,123 @@
         </is>
       </c>
       <c r="B18" t="n">
+        <v>104631.0950484905</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1558.253250006369</v>
+      </c>
+      <c r="D18" t="n">
+        <v>14949.86472154682</v>
+      </c>
+      <c r="E18" t="n">
+        <v>5603.880245002479</v>
+      </c>
+      <c r="F18" t="n">
+        <v>522.793718214301</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1571.51153948007</v>
+      </c>
+      <c r="H18" t="n">
+        <v>93.27272898751208</v>
+      </c>
+      <c r="I18" t="n">
+        <v>7175.391784482549</v>
+      </c>
+      <c r="J18" t="n">
+        <v>616.066447201813</v>
+      </c>
+      <c r="K18" t="n">
+        <v>1065.814462888776</v>
+      </c>
+      <c r="L18" t="n">
+        <v>66.64137275149498</v>
+      </c>
+      <c r="M18" t="n">
+        <v>872.0255065635641</v>
+      </c>
+      <c r="N18" t="n">
+        <v>156.3130690897819</v>
+      </c>
+      <c r="O18" t="n">
+        <v>368.5274226376907</v>
+      </c>
+      <c r="P18" t="n">
         <v>32464.62477656585</v>
       </c>
-      <c r="C18" t="n">
+      <c r="Q18" t="n">
         <v>1917.084750358108</v>
       </c>
-      <c r="D18" t="n">
+      <c r="R18" t="n">
         <v>5720.668541323336</v>
       </c>
-      <c r="E18" t="n">
+      <c r="S18" t="n">
         <v>2298.195199375691</v>
       </c>
-      <c r="F18" t="n">
+      <c r="T18" t="n">
         <v>207.5244364210596</v>
       </c>
-      <c r="G18" t="n">
+      <c r="U18" t="n">
         <v>685.2584542983894</v>
       </c>
-      <c r="H18" t="n">
+      <c r="V18" t="n">
         <v>36.89834281183595</v>
       </c>
-      <c r="I18" t="n">
+      <c r="W18" t="n">
         <v>2983.453653674081</v>
       </c>
-      <c r="J18" t="n">
+      <c r="X18" t="n">
         <v>244.4227792328955</v>
       </c>
-      <c r="K18" t="n">
+      <c r="Y18" t="n">
         <v>328.1650305555928</v>
       </c>
-      <c r="L18" t="n">
+      <c r="Z18" t="n">
         <v>19.13552302802644</v>
       </c>
-      <c r="M18" t="n">
+      <c r="AA18" t="n">
         <v>231.9727766106595</v>
       </c>
-      <c r="N18" t="n">
+      <c r="AB18" t="n">
         <v>36.04145555465609</v>
       </c>
-      <c r="O18" t="n">
+      <c r="AC18" t="n">
         <v>39861.06727929034</v>
       </c>
-      <c r="P18" t="n">
+      <c r="AD18" t="n">
         <v>1990.21486077696</v>
       </c>
-      <c r="Q18" t="n">
+      <c r="AE18" t="n">
         <v>7394.432913796735</v>
       </c>
-      <c r="R18" t="n">
+      <c r="AF18" t="n">
         <v>2824.042567216219</v>
       </c>
-      <c r="S18" t="n">
+      <c r="AG18" t="n">
         <v>257.8007822823</v>
       </c>
-      <c r="T18" t="n">
+      <c r="AH18" t="n">
         <v>772.2808620996474</v>
       </c>
-      <c r="U18" t="n">
+      <c r="AI18" t="n">
         <v>38.75414424911429</v>
       </c>
-      <c r="V18" t="n">
+      <c r="AJ18" t="n">
         <v>3596.323429315867</v>
       </c>
-      <c r="W18" t="n">
+      <c r="AK18" t="n">
         <v>296.5549265314143</v>
       </c>
-      <c r="X18" t="n">
+      <c r="AL18" t="n">
         <v>434.0992711116339</v>
       </c>
-      <c r="Y18" t="n">
+      <c r="AM18" t="n">
         <v>22.32968082193736</v>
       </c>
-      <c r="Z18" t="n">
+      <c r="AN18" t="n">
         <v>322.3668549959459</v>
       </c>
-      <c r="AA18" t="n">
+      <c r="AO18" t="n">
         <v>53.73533695125183</v>
       </c>
     </row>
@@ -2022,81 +2806,123 @@
         </is>
       </c>
       <c r="B19" t="n">
+        <v>99233.95272570745</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1419.771659783246</v>
+      </c>
+      <c r="D19" t="n">
+        <v>13133.40628204136</v>
+      </c>
+      <c r="E19" t="n">
+        <v>4887.994623704785</v>
+      </c>
+      <c r="F19" t="n">
+        <v>479.8737006504808</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1428.050256083153</v>
+      </c>
+      <c r="H19" t="n">
+        <v>84.01543631036621</v>
+      </c>
+      <c r="I19" t="n">
+        <v>6316.044879787938</v>
+      </c>
+      <c r="J19" t="n">
+        <v>563.8891369608471</v>
+      </c>
+      <c r="K19" t="n">
+        <v>1052.363266372928</v>
+      </c>
+      <c r="L19" t="n">
+        <v>62.81985822811413</v>
+      </c>
+      <c r="M19" t="n">
+        <v>868.8097353064428</v>
+      </c>
+      <c r="N19" t="n">
+        <v>145.8090388214638</v>
+      </c>
+      <c r="O19" t="n">
+        <v>358.2311401716157</v>
+      </c>
+      <c r="P19" t="n">
         <v>30119.38859742292</v>
       </c>
-      <c r="C19" t="n">
+      <c r="Q19" t="n">
         <v>1736.66476249109</v>
       </c>
-      <c r="D19" t="n">
+      <c r="R19" t="n">
         <v>4836.715978468995</v>
       </c>
-      <c r="E19" t="n">
+      <c r="S19" t="n">
         <v>1923.973250434202</v>
       </c>
-      <c r="F19" t="n">
+      <c r="T19" t="n">
         <v>179.8137021520933</v>
       </c>
-      <c r="G19" t="n">
+      <c r="U19" t="n">
         <v>611.904366424434</v>
       </c>
-      <c r="H19" t="n">
+      <c r="V19" t="n">
         <v>31.33086458238964</v>
       </c>
-      <c r="I19" t="n">
+      <c r="W19" t="n">
         <v>2535.877616858636</v>
       </c>
-      <c r="J19" t="n">
+      <c r="X19" t="n">
         <v>211.1445667344829</v>
       </c>
-      <c r="K19" t="n">
+      <c r="Y19" t="n">
         <v>316.4643785870497</v>
       </c>
-      <c r="L19" t="n">
+      <c r="Z19" t="n">
         <v>19.39716607790639</v>
       </c>
-      <c r="M19" t="n">
+      <c r="AA19" t="n">
         <v>216.5225582828384</v>
       </c>
-      <c r="N19" t="n">
+      <c r="AB19" t="n">
         <v>31.89491258960997</v>
       </c>
-      <c r="O19" t="n">
+      <c r="AC19" t="n">
         <v>38094.13135671659</v>
       </c>
-      <c r="P19" t="n">
+      <c r="AD19" t="n">
         <v>1851.720301729615</v>
       </c>
-      <c r="Q19" t="n">
+      <c r="AE19" t="n">
         <v>6853.158811800633</v>
       </c>
-      <c r="R19" t="n">
+      <c r="AF19" t="n">
         <v>2581.829539908847</v>
       </c>
-      <c r="S19" t="n">
+      <c r="AG19" t="n">
         <v>252.1425839410952</v>
       </c>
-      <c r="T19" t="n">
+      <c r="AH19" t="n">
         <v>707.9335520738163</v>
       </c>
-      <c r="U19" t="n">
+      <c r="AI19" t="n">
         <v>37.84568357156233</v>
       </c>
-      <c r="V19" t="n">
+      <c r="AJ19" t="n">
         <v>3289.763091982663</v>
       </c>
-      <c r="W19" t="n">
+      <c r="AK19" t="n">
         <v>289.9882675126575</v>
       </c>
-      <c r="X19" t="n">
+      <c r="AL19" t="n">
         <v>437.8126496536024</v>
       </c>
-      <c r="Y19" t="n">
+      <c r="AM19" t="n">
         <v>22.13134435005868</v>
       </c>
-      <c r="Z19" t="n">
+      <c r="AN19" t="n">
         <v>321.762715523745</v>
       </c>
-      <c r="AA19" t="n">
+      <c r="AO19" t="n">
         <v>52.6380912882653</v>
       </c>
     </row>
@@ -2107,81 +2933,123 @@
         </is>
       </c>
       <c r="B20" t="n">
+        <v>100956.0510696426</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1482.556534570725</v>
+      </c>
+      <c r="D20" t="n">
+        <v>13828.19177893497</v>
+      </c>
+      <c r="E20" t="n">
+        <v>5111.492479085098</v>
+      </c>
+      <c r="F20" t="n">
+        <v>489.6370047688469</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1475.223609463987</v>
+      </c>
+      <c r="H20" t="n">
+        <v>87.97960421322621</v>
+      </c>
+      <c r="I20" t="n">
+        <v>6586.716088549086</v>
+      </c>
+      <c r="J20" t="n">
+        <v>577.6166089820731</v>
+      </c>
+      <c r="K20" t="n">
+        <v>1048.396421164467</v>
+      </c>
+      <c r="L20" t="n">
+        <v>65.19308386105459</v>
+      </c>
+      <c r="M20" t="n">
+        <v>854.1204060550322</v>
+      </c>
+      <c r="N20" t="n">
+        <v>154.1121999463859</v>
+      </c>
+      <c r="O20" t="n">
+        <v>364.3812662886295</v>
+      </c>
+      <c r="P20" t="n">
         <v>30156.84747066248</v>
       </c>
-      <c r="C20" t="n">
+      <c r="Q20" t="n">
         <v>1814.044874241087</v>
       </c>
-      <c r="D20" t="n">
+      <c r="R20" t="n">
         <v>4911.175893357597</v>
       </c>
-      <c r="E20" t="n">
+      <c r="S20" t="n">
         <v>1959.178689402509</v>
       </c>
-      <c r="F20" t="n">
+      <c r="T20" t="n">
         <v>183.8348164877708</v>
       </c>
-      <c r="G20" t="n">
+      <c r="U20" t="n">
         <v>655.7587942333535</v>
       </c>
-      <c r="H20" t="n">
+      <c r="V20" t="n">
         <v>33.52550380775735</v>
       </c>
-      <c r="I20" t="n">
+      <c r="W20" t="n">
         <v>2614.937483635863</v>
       </c>
-      <c r="J20" t="n">
+      <c r="X20" t="n">
         <v>217.3603202955282</v>
       </c>
-      <c r="K20" t="n">
+      <c r="Y20" t="n">
         <v>312.2836216826745</v>
       </c>
-      <c r="L20" t="n">
+      <c r="Z20" t="n">
         <v>19.81446849970185</v>
       </c>
-      <c r="M20" t="n">
+      <c r="AA20" t="n">
         <v>217.6542408808185</v>
       </c>
-      <c r="N20" t="n">
+      <c r="AB20" t="n">
         <v>35.81817550107806</v>
       </c>
-      <c r="O20" t="n">
+      <c r="AC20" t="n">
         <v>37572.19880266338</v>
       </c>
-      <c r="P20" t="n">
+      <c r="AD20" t="n">
         <v>1947.71611415023</v>
       </c>
-      <c r="Q20" t="n">
+      <c r="AE20" t="n">
         <v>7220.206106041735</v>
       </c>
-      <c r="R20" t="n">
+      <c r="AF20" t="n">
         <v>2691.761931028316</v>
       </c>
-      <c r="S20" t="n">
+      <c r="AG20" t="n">
         <v>248.4006198059043</v>
       </c>
-      <c r="T20" t="n">
+      <c r="AH20" t="n">
         <v>692.3382162146625</v>
       </c>
-      <c r="U20" t="n">
+      <c r="AI20" t="n">
         <v>37.41803846101172</v>
       </c>
-      <c r="V20" t="n">
+      <c r="AJ20" t="n">
         <v>3384.100147242978</v>
       </c>
-      <c r="W20" t="n">
+      <c r="AK20" t="n">
         <v>285.818658266916</v>
       </c>
-      <c r="X20" t="n">
+      <c r="AL20" t="n">
         <v>414.7442705052798</v>
       </c>
-      <c r="Y20" t="n">
+      <c r="AM20" t="n">
         <v>21.82259785782909</v>
       </c>
-      <c r="Z20" t="n">
+      <c r="AN20" t="n">
         <v>301.9781936940815</v>
       </c>
-      <c r="AA20" t="n">
+      <c r="AO20" t="n">
         <v>50.90108159053389</v>
       </c>
     </row>
@@ -2192,81 +3060,123 @@
         </is>
       </c>
       <c r="B21" t="n">
+        <v>102930.7062141088</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1487.954539101884</v>
+      </c>
+      <c r="D21" t="n">
+        <v>14647.79154167526</v>
+      </c>
+      <c r="E21" t="n">
+        <v>5430.77106792532</v>
+      </c>
+      <c r="F21" t="n">
+        <v>506.0499299327429</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1649.085976140848</v>
+      </c>
+      <c r="H21" t="n">
+        <v>93.06637957797884</v>
+      </c>
+      <c r="I21" t="n">
+        <v>7079.857044066168</v>
+      </c>
+      <c r="J21" t="n">
+        <v>599.1163095107217</v>
+      </c>
+      <c r="K21" t="n">
+        <v>1044.21281390132</v>
+      </c>
+      <c r="L21" t="n">
+        <v>63.45867997284907</v>
+      </c>
+      <c r="M21" t="n">
+        <v>851.1369386284197</v>
+      </c>
+      <c r="N21" t="n">
+        <v>157.1894951697982</v>
+      </c>
+      <c r="O21" t="n">
+        <v>361.8786595276182</v>
+      </c>
+      <c r="P21" t="n">
         <v>35156.95476618902</v>
       </c>
-      <c r="C21" t="n">
+      <c r="Q21" t="n">
         <v>1814.791029582654</v>
       </c>
-      <c r="D21" t="n">
+      <c r="R21" t="n">
         <v>5968.638919531206</v>
       </c>
-      <c r="E21" t="n">
+      <c r="S21" t="n">
         <v>2274.696901113578</v>
       </c>
-      <c r="F21" t="n">
+      <c r="T21" t="n">
         <v>209.3587300746551</v>
       </c>
-      <c r="G21" t="n">
+      <c r="U21" t="n">
         <v>783.5486663241466</v>
       </c>
-      <c r="H21" t="n">
+      <c r="V21" t="n">
         <v>39.46282914811896</v>
       </c>
-      <c r="I21" t="n">
+      <c r="W21" t="n">
         <v>3058.245567437725</v>
       </c>
-      <c r="J21" t="n">
+      <c r="X21" t="n">
         <v>248.8215592227741</v>
       </c>
-      <c r="K21" t="n">
+      <c r="Y21" t="n">
         <v>361.2164668351104</v>
       </c>
-      <c r="L21" t="n">
+      <c r="Z21" t="n">
         <v>21.22087414459916</v>
       </c>
-      <c r="M21" t="n">
+      <c r="AA21" t="n">
         <v>252.8409996131148</v>
       </c>
-      <c r="N21" t="n">
+      <c r="AB21" t="n">
         <v>40.0997764924509</v>
       </c>
-      <c r="O21" t="n">
+      <c r="AC21" t="n">
         <v>35375.18827407724</v>
       </c>
-      <c r="P21" t="n">
+      <c r="AD21" t="n">
         <v>1936.834205860589</v>
       </c>
-      <c r="Q21" t="n">
+      <c r="AE21" t="n">
         <v>6966.144843695444</v>
       </c>
-      <c r="R21" t="n">
+      <c r="AF21" t="n">
         <v>2695.798690905988</v>
       </c>
-      <c r="S21" t="n">
+      <c r="AG21" t="n">
         <v>239.065753471853</v>
       </c>
-      <c r="T21" t="n">
+      <c r="AH21" t="n">
         <v>724.1259617438004</v>
       </c>
-      <c r="U21" t="n">
+      <c r="AI21" t="n">
         <v>36.7165519629629</v>
       </c>
-      <c r="V21" t="n">
+      <c r="AJ21" t="n">
         <v>3419.924652649789</v>
       </c>
-      <c r="W21" t="n">
+      <c r="AK21" t="n">
         <v>275.7823054348158</v>
       </c>
-      <c r="X21" t="n">
+      <c r="AL21" t="n">
         <v>380.8147797481968</v>
       </c>
-      <c r="Y21" t="n">
+      <c r="AM21" t="n">
         <v>20.33850763009366</v>
       </c>
-      <c r="Z21" t="n">
+      <c r="AN21" t="n">
         <v>273.5815285978683</v>
       </c>
-      <c r="AA21" t="n">
+      <c r="AO21" t="n">
         <v>49.8018655397398</v>
       </c>
     </row>

</xml_diff>